<commit_message>
Tests on graphs with dNN only
</commit_message>
<xml_diff>
--- a/results_table.xlsx
+++ b/results_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arteger\Desktop\masters_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD989EC-059A-41CC-9BB3-937547DD4707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380B3572-7670-4BCA-9DFE-FE8B301B7D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A2B8B723-FC77-40CE-AF1D-99DBE66D63C9}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>Edges</t>
   </si>
   <si>
-    <t>Solo no complement dNN result</t>
-  </si>
-  <si>
     <t>Erdos-Renyi</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>Sometimes it finds correct MIS, sometimes zero</t>
+  </si>
+  <si>
+    <t>Only no complement dNN result</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,12 +484,12 @@
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>200</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>250</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>250</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>350</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>350</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>200</v>
@@ -731,12 +731,12 @@
         <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>200</v>
@@ -784,12 +784,12 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>7115</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>1000</v>
@@ -815,7 +815,7 @@
         <v>49421</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18">
         <v>53</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>125</v>
@@ -835,7 +835,7 @@
         <v>787</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19">
         <v>32</v>

</xml_diff>